<commit_message>
Maj du Backlog + Supression gestion de l'excel
</commit_message>
<xml_diff>
--- a/BackLogFonctionnalité.xlsx
+++ b/BackLogFonctionnalité.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Description</t>
   </si>
@@ -35,12 +35,6 @@
     <t>Etat</t>
   </si>
   <si>
-    <t>importer des notes à partir d'un fichier excel</t>
-  </si>
-  <si>
-    <t>Analyser le fichier excel</t>
-  </si>
-  <si>
     <t>Créer des groupes de modules</t>
   </si>
   <si>
@@ -60,14 +54,75 @@
   </si>
   <si>
     <t>Permettre de générer un avis général</t>
+  </si>
+  <si>
+    <t>Lot</t>
+  </si>
+  <si>
+    <t>Convertir des fichiers Excel en csv</t>
+  </si>
+  <si>
+    <t>Gestion du csv :</t>
+  </si>
+  <si>
+    <t>Gestion de module :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion des avis : </t>
+  </si>
+  <si>
+    <t>Gestion des données :</t>
+  </si>
+  <si>
+    <t>Traiter les données du csv</t>
+  </si>
+  <si>
+    <t>Génération de pdf</t>
+  </si>
+  <si>
+    <t>Ecriture dans un fichier des données pour enregistrer</t>
+  </si>
+  <si>
+    <t>importer les données à partir d'un fichier csv</t>
+  </si>
+  <si>
+    <t>Mise en place de la structure :</t>
+  </si>
+  <si>
+    <t>Implémenter les modules</t>
+  </si>
+  <si>
+    <t>Implémenter les étudiants</t>
+  </si>
+  <si>
+    <t>Implémenter les groupes de modules</t>
+  </si>
+  <si>
+    <t>Interface Homme-Machine :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,8 +150,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -385,66 +443,197 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>